<commit_message>
commit chnages in Weekly task sheet file
commit chnages in Weekly task sheet file
</commit_message>
<xml_diff>
--- a/WeeklyTaskSheet_Feb2021.xlsx
+++ b/WeeklyTaskSheet_Feb2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ImportantFiles\TaskList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OptumRepository\OPTUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FA423A-FE16-40E2-9F23-D95D5E201B14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE47EAA-B118-48A0-AA3E-8B103ED977CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4F434F4A-D07B-4503-A18F-3AC92A18487C}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="10920" xr2:uid="{4F434F4A-D07B-4503-A18F-3AC92A18487C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1390,7 +1390,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,8 +1796,8 @@
       <c r="D19" t="s">
         <v>283</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>249</v>
+      <c r="E19" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F19" t="s">
         <v>251</v>

</xml_diff>